<commit_message>
add comments and initiate CSS
</commit_message>
<xml_diff>
--- a/documents/Tischplatten_Berechnungsgrundlage.xlsx
+++ b/documents/Tischplatten_Berechnungsgrundlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\webentwicklung\javascript\_projekte\tischplatten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\iad-js-kurs\projekt-tischplatten\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AEDBE0-712B-426C-8954-1EBE27470A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14B5375-120E-404D-BCDA-EB24AB575565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6735F5B-8943-4856-9AAA-08D8BB47D687}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6735F5B-8943-4856-9AAA-08D8BB47D687}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -304,11 +304,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;mm&quot;"/>
     <numFmt numFmtId="166" formatCode="0\ &quot;cm&quot;"/>
-    <numFmt numFmtId="168" formatCode="General\ &quot;m²&quot;"/>
+    <numFmt numFmtId="167" formatCode="General\ &quot;m²&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -904,7 +905,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -921,21 +922,11 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -946,8 +937,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -960,56 +949,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1019,54 +972,6 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1114,18 +1019,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="5" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="9" fillId="8" borderId="5" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Ausgabe" xfId="4" builtinId="21"/>
-    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="3" builtinId="15"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="3" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2294,9 +2294,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2334,7 +2334,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2440,7 +2440,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2582,7 +2582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2590,13 +2590,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECF9E65-F32C-4014-A5B3-983E5EEF0270}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
@@ -2611,49 +2611,49 @@
     <col min="12" max="12" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="39" customFormat="1" ht="18.75">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="18.75">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="36" t="s">
+      <c r="E1" s="116"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="117"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="34"/>
-    </row>
-    <row r="2" spans="1:12" s="47" customFormat="1" ht="48" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="K1" s="118"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="1:12" s="32" customFormat="1" ht="48" customHeight="1">
+      <c r="A2" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="110"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="44" t="s">
+      <c r="E2" s="112"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46" t="s">
+      <c r="H2" s="113"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="41"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:12" ht="75" customHeight="1">
       <c r="A3" t="s">
@@ -2672,7 +2672,7 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="59.25" customHeight="1" thickBot="1">
@@ -2693,7 +2693,7 @@
       <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="2"/>
@@ -2723,7 +2723,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="33" t="s">
         <v>45</v>
       </c>
       <c r="F6" s="2"/>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="48" t="s">
+      <c r="J6" s="33" t="s">
         <v>46</v>
       </c>
       <c r="L6" s="2"/>
@@ -2804,59 +2804,59 @@
       <c r="L12" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="23.25">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="23"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
-      <c r="G16" s="123" t="s">
+      <c r="G16" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="123"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="124"/>
-      <c r="K16" s="124"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.75">
-      <c r="G18" s="27" t="s">
+      <c r="H16" s="109"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75">
+      <c r="G18" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="28"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75">
-      <c r="G19" s="29" t="s">
+      <c r="H18" s="120"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75">
+      <c r="G19" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="25" t="s">
         <v>29</v>
       </c>
       <c r="K19" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75">
+    <row r="20" spans="1:14" ht="15.75">
       <c r="G20" s="6">
         <v>180</v>
       </c>
       <c r="H20" s="6">
         <v>230</v>
       </c>
-      <c r="J20" s="125">
+      <c r="J20" s="89">
         <f>$G$20/100*$H$20/100</f>
         <v>4.1399999999999997</v>
       </c>
@@ -2864,653 +2864,675 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18.75">
-      <c r="D22" s="12" t="s">
+    <row r="22" spans="1:14" ht="18.75">
+      <c r="D22" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="G22" s="12" t="s">
+      <c r="E22" s="122"/>
+      <c r="G22" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" spans="1:11" ht="75">
+      <c r="H22" s="123"/>
+      <c r="I22" s="123"/>
+      <c r="J22" s="123"/>
+      <c r="K22" s="122"/>
+    </row>
+    <row r="23" spans="1:14" ht="75">
       <c r="A23" s="4"/>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="85" t="s">
+      <c r="E23" s="51" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="14" t="str">
+      <c r="G23" s="12" t="str">
         <f>"Preis / m² * "&amp;J20&amp;" m²"</f>
         <v>Preis / m² * 4,14 m²</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="17" t="s">
+      <c r="I23" s="1"/>
+      <c r="J23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1">
-      <c r="A24" s="50" t="s">
+    <row r="24" spans="1:14" ht="15" customHeight="1">
+      <c r="A24" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="56">
+      <c r="B24" s="92"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="38">
         <v>25</v>
       </c>
-      <c r="E24" s="86">
+      <c r="E24" s="52">
         <v>300</v>
       </c>
-      <c r="F24" s="76"/>
-      <c r="G24" s="94">
+      <c r="F24" s="42"/>
+      <c r="G24" s="60">
         <f t="shared" ref="G24:G34" si="0">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*E24*(1+$K$20),$G$20/100*$H$20/100*E24)</f>
         <v>1242</v>
       </c>
-      <c r="H24" s="95">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$50))</f>
+      <c r="H24" s="61">
+        <f t="shared" ref="H24:H34" si="1">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$50))</f>
         <v>1439.0640000000001</v>
       </c>
-      <c r="I24" s="96"/>
-      <c r="J24" s="95">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$53))</f>
+      <c r="I24" s="62"/>
+      <c r="J24" s="61">
+        <f t="shared" ref="J24:J34" si="2">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$53))</f>
         <v>1537.5959999999998</v>
       </c>
-      <c r="K24" s="86">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$50+$D$53))</f>
+      <c r="K24" s="52">
+        <f t="shared" ref="K24:K34" si="3">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E24+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E24+$D$50+$D$53))</f>
         <v>1734.6599999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="57">
+      <c r="M24" s="124"/>
+      <c r="N24" s="124"/>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1">
+      <c r="A25" s="94"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="39">
         <v>30</v>
       </c>
-      <c r="E25" s="87">
+      <c r="E25" s="53">
         <v>360</v>
       </c>
-      <c r="F25" s="77"/>
-      <c r="G25" s="97">
+      <c r="F25" s="43"/>
+      <c r="G25" s="63">
         <f t="shared" si="0"/>
         <v>1490.3999999999999</v>
       </c>
-      <c r="H25" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E25+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E25+$D$50))</f>
+      <c r="H25" s="64">
+        <f t="shared" si="1"/>
         <v>1687.4639999999999</v>
       </c>
-      <c r="I25" s="99"/>
-      <c r="J25" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E25+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E25+$D$53))</f>
+      <c r="I25" s="65"/>
+      <c r="J25" s="64">
+        <f t="shared" si="2"/>
         <v>1785.9959999999999</v>
       </c>
-      <c r="K25" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E25+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E25+$D$50+$D$53))</f>
+      <c r="K25" s="53">
+        <f t="shared" si="3"/>
         <v>1983.06</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="57">
+      <c r="M25" s="124"/>
+      <c r="N25" s="124"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1">
+      <c r="A26" s="94"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="39">
         <v>40</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="53">
         <v>420</v>
       </c>
-      <c r="F26" s="77"/>
-      <c r="G26" s="97">
+      <c r="F26" s="43"/>
+      <c r="G26" s="63">
         <f t="shared" si="0"/>
         <v>1738.8</v>
       </c>
-      <c r="H26" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E26+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E26+$D$50))</f>
+      <c r="H26" s="64">
+        <f t="shared" si="1"/>
         <v>1935.864</v>
       </c>
-      <c r="I26" s="99"/>
-      <c r="J26" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E26+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E26+$D$53))</f>
+      <c r="I26" s="65"/>
+      <c r="J26" s="64">
+        <f t="shared" si="2"/>
         <v>2034.3959999999997</v>
       </c>
-      <c r="K26" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E26+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E26+$D$50+$D$53))</f>
+      <c r="K26" s="53">
+        <f t="shared" si="3"/>
         <v>2231.46</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="62"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="58">
+      <c r="M26" s="124"/>
+      <c r="N26" s="124"/>
+    </row>
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="94"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="40">
         <v>50</v>
       </c>
-      <c r="E27" s="88">
+      <c r="E27" s="54">
         <v>480</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="100">
+      <c r="F27" s="44"/>
+      <c r="G27" s="66">
         <f t="shared" si="0"/>
         <v>1987.1999999999998</v>
       </c>
-      <c r="H27" s="101">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E27+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E27+$D$50))</f>
+      <c r="H27" s="67">
+        <f t="shared" si="1"/>
         <v>2184.2640000000001</v>
       </c>
-      <c r="I27" s="102"/>
-      <c r="J27" s="101">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E27+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E27+$D$53))</f>
+      <c r="I27" s="68"/>
+      <c r="J27" s="67">
+        <f t="shared" si="2"/>
         <v>2282.7959999999998</v>
       </c>
-      <c r="K27" s="88">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E27+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E27+$D$50+$D$53))</f>
+      <c r="K27" s="54">
+        <f t="shared" si="3"/>
         <v>2479.8599999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1">
-      <c r="A28" s="62"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="57">
+      <c r="M27" s="124"/>
+      <c r="N27" s="124"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1">
+      <c r="A28" s="94"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="39">
         <v>60</v>
       </c>
-      <c r="E28" s="87">
+      <c r="E28" s="53">
         <v>560</v>
       </c>
-      <c r="F28" s="77"/>
-      <c r="G28" s="97">
+      <c r="F28" s="43"/>
+      <c r="G28" s="63">
         <f t="shared" si="0"/>
         <v>2318.3999999999996</v>
       </c>
-      <c r="H28" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E28+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E28+$D$50))</f>
+      <c r="H28" s="64">
+        <f t="shared" si="1"/>
         <v>2515.4639999999999</v>
       </c>
-      <c r="I28" s="99"/>
-      <c r="J28" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E28+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E28+$D$53))</f>
+      <c r="I28" s="65"/>
+      <c r="J28" s="64">
+        <f t="shared" si="2"/>
         <v>2613.9959999999996</v>
       </c>
-      <c r="K28" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E28+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E28+$D$50+$D$53))</f>
+      <c r="K28" s="53">
+        <f t="shared" si="3"/>
         <v>2811.06</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1">
-      <c r="A29" s="62"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="57">
+      <c r="M28" s="124"/>
+      <c r="N28" s="124"/>
+    </row>
+    <row r="29" spans="1:14" ht="15" customHeight="1">
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="39">
         <v>70</v>
       </c>
-      <c r="E29" s="87">
+      <c r="E29" s="53">
         <v>640</v>
       </c>
-      <c r="F29" s="77"/>
-      <c r="G29" s="97">
+      <c r="F29" s="43"/>
+      <c r="G29" s="63">
         <f t="shared" si="0"/>
         <v>2649.6</v>
       </c>
-      <c r="H29" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E29+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E29+$D$50))</f>
+      <c r="H29" s="64">
+        <f t="shared" si="1"/>
         <v>2846.6639999999998</v>
       </c>
-      <c r="I29" s="99"/>
-      <c r="J29" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E29+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E29+$D$53))</f>
+      <c r="I29" s="65"/>
+      <c r="J29" s="64">
+        <f t="shared" si="2"/>
         <v>2945.1959999999995</v>
       </c>
-      <c r="K29" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E29+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E29+$D$50+$D$53))</f>
+      <c r="K29" s="53">
+        <f t="shared" si="3"/>
         <v>3142.2599999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1">
-      <c r="A30" s="62"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="57">
+      <c r="M29" s="124"/>
+      <c r="N29" s="124"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1">
+      <c r="A30" s="94"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="39">
         <v>80</v>
       </c>
-      <c r="E30" s="87">
+      <c r="E30" s="53">
         <v>720</v>
       </c>
-      <c r="F30" s="77"/>
-      <c r="G30" s="97">
+      <c r="F30" s="43"/>
+      <c r="G30" s="63">
         <f t="shared" si="0"/>
         <v>2980.7999999999997</v>
       </c>
-      <c r="H30" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E30+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E30+$D$50))</f>
+      <c r="H30" s="64">
+        <f t="shared" si="1"/>
         <v>3177.864</v>
       </c>
-      <c r="I30" s="99"/>
-      <c r="J30" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E30+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E30+$D$53))</f>
+      <c r="I30" s="65"/>
+      <c r="J30" s="64">
+        <f t="shared" si="2"/>
         <v>3276.3959999999997</v>
       </c>
-      <c r="K30" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E30+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E30+$D$50+$D$53))</f>
+      <c r="K30" s="53">
+        <f t="shared" si="3"/>
         <v>3473.4599999999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1">
-      <c r="A31" s="62"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="57">
+      <c r="M30" s="124"/>
+      <c r="N30" s="124"/>
+    </row>
+    <row r="31" spans="1:14" ht="15" customHeight="1">
+      <c r="A31" s="94"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="39">
         <v>90</v>
       </c>
-      <c r="E31" s="87">
+      <c r="E31" s="53">
         <v>800</v>
       </c>
-      <c r="F31" s="77"/>
-      <c r="G31" s="97">
+      <c r="F31" s="43"/>
+      <c r="G31" s="63">
         <f t="shared" si="0"/>
         <v>3311.9999999999995</v>
       </c>
-      <c r="H31" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E31+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E31+$D$50))</f>
+      <c r="H31" s="64">
+        <f t="shared" si="1"/>
         <v>3509.0639999999999</v>
       </c>
-      <c r="I31" s="99"/>
-      <c r="J31" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E31+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E31+$D$53))</f>
+      <c r="I31" s="65"/>
+      <c r="J31" s="64">
+        <f t="shared" si="2"/>
         <v>3607.5959999999995</v>
       </c>
-      <c r="K31" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E31+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E31+$D$50+$D$53))</f>
+      <c r="K31" s="53">
+        <f t="shared" si="3"/>
         <v>3804.66</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="15" customHeight="1">
-      <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="57">
+      <c r="M31" s="124"/>
+      <c r="N31" s="124"/>
+    </row>
+    <row r="32" spans="1:14" ht="15" customHeight="1">
+      <c r="A32" s="94"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="39">
         <v>100</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="53">
         <v>880</v>
       </c>
-      <c r="F32" s="77"/>
-      <c r="G32" s="97">
+      <c r="F32" s="43"/>
+      <c r="G32" s="63">
         <f t="shared" si="0"/>
         <v>3643.2</v>
       </c>
-      <c r="H32" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E32+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E32+$D$50))</f>
+      <c r="H32" s="64">
+        <f t="shared" si="1"/>
         <v>3840.2639999999997</v>
       </c>
-      <c r="I32" s="99"/>
-      <c r="J32" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E32+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E32+$D$53))</f>
+      <c r="I32" s="65"/>
+      <c r="J32" s="64">
+        <f t="shared" si="2"/>
         <v>3938.7959999999998</v>
       </c>
-      <c r="K32" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E32+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E32+$D$50+$D$53))</f>
+      <c r="K32" s="53">
+        <f t="shared" si="3"/>
         <v>4135.8599999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1">
-      <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="57">
+      <c r="M32" s="124"/>
+      <c r="N32" s="124"/>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1">
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="39">
         <v>110</v>
       </c>
-      <c r="E33" s="87">
+      <c r="E33" s="53">
         <v>960</v>
       </c>
-      <c r="F33" s="77"/>
-      <c r="G33" s="97">
+      <c r="F33" s="43"/>
+      <c r="G33" s="63">
         <f t="shared" si="0"/>
         <v>3974.3999999999996</v>
       </c>
-      <c r="H33" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E33+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E33+$D$50))</f>
+      <c r="H33" s="64">
+        <f t="shared" si="1"/>
         <v>4171.4639999999999</v>
       </c>
-      <c r="I33" s="99"/>
-      <c r="J33" s="98">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E33+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E33+$D$53))</f>
+      <c r="I33" s="65"/>
+      <c r="J33" s="64">
+        <f t="shared" si="2"/>
         <v>4269.9960000000001</v>
       </c>
-      <c r="K33" s="87">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E33+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E33+$D$50+$D$53))</f>
+      <c r="K33" s="53">
+        <f t="shared" si="3"/>
         <v>4467.0599999999995</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1">
-      <c r="A34" s="65"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="59">
+      <c r="M33" s="124"/>
+      <c r="N33" s="124"/>
+    </row>
+    <row r="34" spans="1:14" ht="15" customHeight="1">
+      <c r="A34" s="97"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="41">
         <v>120</v>
       </c>
-      <c r="E34" s="89">
+      <c r="E34" s="55">
         <v>1040</v>
       </c>
-      <c r="F34" s="83"/>
-      <c r="G34" s="103">
+      <c r="F34" s="49"/>
+      <c r="G34" s="69">
         <f t="shared" si="0"/>
         <v>4305.5999999999995</v>
       </c>
-      <c r="H34" s="104">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E34+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E34+$D$50))</f>
+      <c r="H34" s="70">
+        <f t="shared" si="1"/>
         <v>4502.6639999999989</v>
       </c>
-      <c r="I34" s="105"/>
-      <c r="J34" s="104">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E34+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E34+$D$53))</f>
+      <c r="I34" s="71"/>
+      <c r="J34" s="70">
+        <f t="shared" si="2"/>
         <v>4601.1959999999999</v>
       </c>
-      <c r="K34" s="89">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E34+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E34+$D$50+$D$53))</f>
+      <c r="K34" s="55">
+        <f t="shared" si="3"/>
         <v>4798.2599999999993</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="D35" s="118"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="24"/>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="M34" s="124"/>
+      <c r="N34" s="124"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="D35" s="84"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="20"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="4"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="15"/>
-    </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1">
-      <c r="A37" s="51" t="s">
+      <c r="D36" s="86"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" ht="15" customHeight="1">
+      <c r="A37" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="52">
+      <c r="B37" s="101"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="34">
         <v>40</v>
       </c>
-      <c r="E37" s="90">
+      <c r="E37" s="56">
         <v>315</v>
       </c>
-      <c r="F37" s="80"/>
-      <c r="G37" s="106">
-        <f t="shared" ref="G37:G45" si="1">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*E37*(1+$K$20),$G$20/100*$H$20/100*E37)</f>
+      <c r="F37" s="46"/>
+      <c r="G37" s="72">
+        <f t="shared" ref="G37:G45" si="4">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*E37*(1+$K$20),$G$20/100*$H$20/100*E37)</f>
         <v>1304.0999999999999</v>
       </c>
-      <c r="H37" s="107">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$50))</f>
+      <c r="H37" s="73">
+        <f t="shared" ref="H37:H45" si="5">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$50))</f>
         <v>1501.164</v>
       </c>
-      <c r="I37" s="108"/>
-      <c r="J37" s="107">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$53))</f>
+      <c r="I37" s="74"/>
+      <c r="J37" s="73">
+        <f t="shared" ref="J37:J45" si="6">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$53))</f>
         <v>1599.6959999999997</v>
       </c>
-      <c r="K37" s="90">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$50+$D$53))</f>
+      <c r="K37" s="56">
+        <f t="shared" ref="K37:K45" si="7">IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E37+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E37+$D$50+$D$53))</f>
         <v>1796.7599999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="70"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="53">
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A38" s="103"/>
+      <c r="B38" s="104"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="35">
         <v>50</v>
       </c>
-      <c r="E38" s="91">
+      <c r="E38" s="57">
         <v>360</v>
       </c>
-      <c r="F38" s="81"/>
-      <c r="G38" s="109">
-        <f t="shared" si="1"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="75">
+        <f t="shared" si="4"/>
         <v>1490.3999999999999</v>
       </c>
-      <c r="H38" s="110">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E38+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E38+$D$50))</f>
+      <c r="H38" s="76">
+        <f t="shared" si="5"/>
         <v>1687.4639999999999</v>
       </c>
-      <c r="I38" s="111"/>
-      <c r="J38" s="110">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E38+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E38+$D$53))</f>
+      <c r="I38" s="77"/>
+      <c r="J38" s="76">
+        <f t="shared" si="6"/>
         <v>1785.9959999999999</v>
       </c>
-      <c r="K38" s="91">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E38+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E38+$D$50+$D$53))</f>
+      <c r="K38" s="57">
+        <f t="shared" si="7"/>
         <v>1983.06</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1">
-      <c r="A39" s="70"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="54">
+    <row r="39" spans="1:14" ht="15" customHeight="1">
+      <c r="A39" s="103"/>
+      <c r="B39" s="104"/>
+      <c r="C39" s="105"/>
+      <c r="D39" s="36">
         <v>60</v>
       </c>
-      <c r="E39" s="92">
+      <c r="E39" s="58">
         <v>420</v>
       </c>
-      <c r="F39" s="80"/>
-      <c r="G39" s="112">
-        <f t="shared" si="1"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="78">
+        <f t="shared" si="4"/>
         <v>1738.8</v>
       </c>
-      <c r="H39" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E39+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E39+$D$50))</f>
+      <c r="H39" s="79">
+        <f t="shared" si="5"/>
         <v>1935.864</v>
       </c>
-      <c r="I39" s="114"/>
-      <c r="J39" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E39+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E39+$D$53))</f>
+      <c r="I39" s="80"/>
+      <c r="J39" s="79">
+        <f t="shared" si="6"/>
         <v>2034.3959999999997</v>
       </c>
-      <c r="K39" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E39+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E39+$D$50+$D$53))</f>
+      <c r="K39" s="58">
+        <f t="shared" si="7"/>
         <v>2231.46</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1">
-      <c r="A40" s="70"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="54">
+    <row r="40" spans="1:14" ht="15" customHeight="1">
+      <c r="A40" s="103"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="36">
         <v>70</v>
       </c>
-      <c r="E40" s="92">
+      <c r="E40" s="58">
         <v>480</v>
       </c>
-      <c r="F40" s="80"/>
-      <c r="G40" s="112">
-        <f t="shared" si="1"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="78">
+        <f t="shared" si="4"/>
         <v>1987.1999999999998</v>
       </c>
-      <c r="H40" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E40+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E40+$D$50))</f>
+      <c r="H40" s="79">
+        <f t="shared" si="5"/>
         <v>2184.2640000000001</v>
       </c>
-      <c r="I40" s="114"/>
-      <c r="J40" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E40+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E40+$D$53))</f>
+      <c r="I40" s="80"/>
+      <c r="J40" s="79">
+        <f t="shared" si="6"/>
         <v>2282.7959999999998</v>
       </c>
-      <c r="K40" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E40+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E40+$D$50+$D$53))</f>
+      <c r="K40" s="58">
+        <f t="shared" si="7"/>
         <v>2479.8599999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1">
-      <c r="A41" s="70"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="54">
+    <row r="41" spans="1:14" ht="15" customHeight="1">
+      <c r="A41" s="103"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="105"/>
+      <c r="D41" s="36">
         <v>80</v>
       </c>
-      <c r="E41" s="92">
+      <c r="E41" s="58">
         <v>540</v>
       </c>
-      <c r="F41" s="80"/>
-      <c r="G41" s="112">
-        <f t="shared" si="1"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="78">
+        <f t="shared" si="4"/>
         <v>2235.6</v>
       </c>
-      <c r="H41" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E41+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E41+$D$50))</f>
+      <c r="H41" s="79">
+        <f t="shared" si="5"/>
         <v>2432.6639999999998</v>
       </c>
-      <c r="I41" s="114"/>
-      <c r="J41" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E41+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E41+$D$53))</f>
+      <c r="I41" s="80"/>
+      <c r="J41" s="79">
+        <f t="shared" si="6"/>
         <v>2531.1959999999999</v>
       </c>
-      <c r="K41" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E41+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E41+$D$50+$D$53))</f>
+      <c r="K41" s="58">
+        <f t="shared" si="7"/>
         <v>2728.2599999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1">
-      <c r="A42" s="70"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="54">
+    <row r="42" spans="1:14" ht="15" customHeight="1">
+      <c r="A42" s="103"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="105"/>
+      <c r="D42" s="36">
         <v>90</v>
       </c>
-      <c r="E42" s="92">
+      <c r="E42" s="58">
         <v>600</v>
       </c>
-      <c r="F42" s="80"/>
-      <c r="G42" s="112">
-        <f t="shared" si="1"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="78">
+        <f t="shared" si="4"/>
         <v>2484</v>
       </c>
-      <c r="H42" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E42+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E42+$D$50))</f>
+      <c r="H42" s="79">
+        <f t="shared" si="5"/>
         <v>2681.0639999999999</v>
       </c>
-      <c r="I42" s="114"/>
-      <c r="J42" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E42+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E42+$D$53))</f>
+      <c r="I42" s="80"/>
+      <c r="J42" s="79">
+        <f t="shared" si="6"/>
         <v>2779.5959999999995</v>
       </c>
-      <c r="K42" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E42+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E42+$D$50+$D$53))</f>
+      <c r="K42" s="58">
+        <f t="shared" si="7"/>
         <v>2976.66</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1">
-      <c r="A43" s="70"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="54">
+    <row r="43" spans="1:14" ht="15" customHeight="1">
+      <c r="A43" s="103"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="36">
         <v>100</v>
       </c>
-      <c r="E43" s="92">
+      <c r="E43" s="58">
         <v>660</v>
       </c>
-      <c r="F43" s="80"/>
-      <c r="G43" s="112">
-        <f t="shared" si="1"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="78">
+        <f t="shared" si="4"/>
         <v>2732.3999999999996</v>
       </c>
-      <c r="H43" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E43+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E43+$D$50))</f>
+      <c r="H43" s="79">
+        <f t="shared" si="5"/>
         <v>2929.4639999999999</v>
       </c>
-      <c r="I43" s="114"/>
-      <c r="J43" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E43+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E43+$D$53))</f>
+      <c r="I43" s="80"/>
+      <c r="J43" s="79">
+        <f t="shared" si="6"/>
         <v>3027.9959999999996</v>
       </c>
-      <c r="K43" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E43+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E43+$D$50+$D$53))</f>
+      <c r="K43" s="58">
+        <f t="shared" si="7"/>
         <v>3225.06</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="72"/>
-      <c r="D44" s="54">
+    <row r="44" spans="1:14" ht="15" customHeight="1">
+      <c r="A44" s="103"/>
+      <c r="B44" s="104"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="36">
         <v>110</v>
       </c>
-      <c r="E44" s="92">
+      <c r="E44" s="58">
         <v>720</v>
       </c>
-      <c r="F44" s="80"/>
-      <c r="G44" s="112">
-        <f t="shared" si="1"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="78">
+        <f t="shared" si="4"/>
         <v>2980.7999999999997</v>
       </c>
-      <c r="H44" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E44+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E44+$D$50))</f>
+      <c r="H44" s="79">
+        <f t="shared" si="5"/>
         <v>3177.864</v>
       </c>
-      <c r="I44" s="114"/>
-      <c r="J44" s="113">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E44+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E44+$D$53))</f>
+      <c r="I44" s="80"/>
+      <c r="J44" s="79">
+        <f t="shared" si="6"/>
         <v>3276.3959999999997</v>
       </c>
-      <c r="K44" s="92">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E44+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E44+$D$50+$D$53))</f>
+      <c r="K44" s="58">
+        <f t="shared" si="7"/>
         <v>3473.4599999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" customHeight="1">
-      <c r="A45" s="73"/>
-      <c r="B45" s="74"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="55">
+    <row r="45" spans="1:14" ht="15" customHeight="1">
+      <c r="A45" s="106"/>
+      <c r="B45" s="107"/>
+      <c r="C45" s="108"/>
+      <c r="D45" s="37">
         <v>120</v>
       </c>
-      <c r="E45" s="93">
+      <c r="E45" s="59">
         <v>780</v>
       </c>
-      <c r="F45" s="82"/>
-      <c r="G45" s="115">
-        <f t="shared" si="1"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="81">
+        <f t="shared" si="4"/>
         <v>3229.2</v>
       </c>
-      <c r="H45" s="116">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E45+$D$50)*(1+$K$20),$G$20/100*$H$20/100*(E45+$D$50))</f>
+      <c r="H45" s="82">
+        <f t="shared" si="5"/>
         <v>3426.2639999999997</v>
       </c>
-      <c r="I45" s="117"/>
-      <c r="J45" s="116">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E45+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E45+$D$53))</f>
+      <c r="I45" s="83"/>
+      <c r="J45" s="82">
+        <f t="shared" si="6"/>
         <v>3524.7959999999998</v>
       </c>
-      <c r="K45" s="93">
-        <f>IF($G$20/100*$H$20/100&lt;1,$G$20/100*$H$20/100*(E45+$D$50+$D$53)*(1+$K$20),$G$20/100*$H$20/100*(E45+$D$50+$D$53))</f>
+      <c r="K45" s="59">
+        <f t="shared" si="7"/>
         <v>3721.8599999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="122">
+    <row r="47" spans="1:14">
+      <c r="A47" s="88">
         <v>4500</v>
       </c>
-      <c r="B47" s="122">
+      <c r="B47" s="88">
         <v>1800</v>
       </c>
     </row>
@@ -3542,6 +3564,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A24:C34"/>
     <mergeCell ref="A37:C45"/>
@@ -3550,11 +3577,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="G18:H18"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:K22"/>
   </mergeCells>

</xml_diff>